<commit_message>
Working with declaration pages
</commit_message>
<xml_diff>
--- a/Here are the errors.xlsx
+++ b/Here are the errors.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A6:B268"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,10 +421,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
-          <t>068-TK-TBA TK</t>
+          <t>Chantier__002-TK-HTC TK</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Chantier__002-TK-HTC TK converted successfully :)</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>Chantier__NCC-TK-183 TK</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>Chantier__NCC-TK-183 TK converted successfully :)</t>
         </is>
       </c>
     </row>

</xml_diff>